<commit_message>
Modified diffomega <= 0.1
</commit_message>
<xml_diff>
--- a/Mathieusche Differentialgleichung/Programme/dataFolder/dataFolder_Arnold_Excel_Classic_Symmetric_test/STRUTTscheKarte_D1dot5e-01_SW1dot0e-01_unt0CharExAll.xlsx
+++ b/Mathieusche Differentialgleichung/Programme/dataFolder/dataFolder_Arnold_Excel_Classic_Symmetric_test/STRUTTscheKarte_D1dot5e-01_SW1dot0e-01_unt0CharExAll.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="80" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="110" uniqueCount="10">
   <si>
     <t>nu02</t>
   </si>
@@ -531,7 +531,7 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="C14" s="0">
-        <v>-0.28746830727795914</v>
+        <v>-0.28746830727795908</v>
       </c>
       <c r="D14" s="0">
         <v>-0.01253169273031411</v>
@@ -595,7 +595,7 @@
         <v>1.4000000000000001</v>
       </c>
       <c r="C16" s="0">
-        <v>-0.26789316527092838</v>
+        <v>-0.26789316527092844</v>
       </c>
       <c r="D16" s="0">
         <v>-0.032106834738656505</v>
@@ -1683,7 +1683,7 @@
         <v>4.8000000000000007</v>
       </c>
       <c r="C50" s="0">
-        <v>-0.28592209889802606</v>
+        <v>-0.28592209889802611</v>
       </c>
       <c r="D50" s="0">
         <v>-0.014077901120465294</v>
@@ -1715,7 +1715,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="C51" s="0">
-        <v>-0.28908734234778027</v>
+        <v>-0.28908734234778033</v>
       </c>
       <c r="D51" s="0">
         <v>-0.010912657671058434</v>
@@ -1747,7 +1747,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="0">
-        <v>-0.28850306631269762</v>
+        <v>-0.28850306631269756</v>
       </c>
       <c r="D52" s="0">
         <v>-0.011496933706512606</v>
@@ -1910,7 +1910,7 @@
         <v>-0.21156827611741144</v>
       </c>
       <c r="D57" s="0">
-        <v>-0.088431723903173346</v>
+        <v>-0.088431723903173359</v>
       </c>
       <c r="E57" s="0">
         <v>-2</v>
@@ -2291,10 +2291,10 @@
         <v>6.7000000000000002</v>
       </c>
       <c r="C69" s="0">
-        <v>-0.15000000001108615</v>
+        <v>-0.15000000001108618</v>
       </c>
       <c r="D69" s="0">
-        <v>-0.15000000001108615</v>
+        <v>-0.15000000001108618</v>
       </c>
       <c r="E69" s="0">
         <v>-2.3473570282268783</v>

</xml_diff>

<commit_message>
Comparison between methods from Arnold and Peters for calculation of char. exponent
</commit_message>
<xml_diff>
--- a/Mathieusche Differentialgleichung/Programme/dataFolder/dataFolder_Arnold_Excel_Classic_Symmetric_test/STRUTTscheKarte_D1dot5e-01_SW1dot0e-01_unt0CharExAll.xlsx
+++ b/Mathieusche Differentialgleichung/Programme/dataFolder/dataFolder_Arnold_Excel_Classic_Symmetric_test/STRUTTscheKarte_D1dot5e-01_SW1dot0e-01_unt0CharExAll.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="110" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="121" uniqueCount="11">
   <si>
     <t>nu02</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>ImagCharExp2</t>
+  </si>
+  <si>
+    <t>ImagEigNoadditionfactor</t>
   </si>
 </sst>
 </file>
@@ -89,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:K92"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -101,10 +104,11 @@
     <col min="4" max="4" width="14.21875" customWidth="true"/>
     <col min="5" max="5" width="13.21875" customWidth="true"/>
     <col min="6" max="6" width="12.5546875" customWidth="true"/>
-    <col min="7" max="7" width="14.5546875" customWidth="true"/>
-    <col min="8" max="8" width="14.21875" customWidth="true"/>
-    <col min="9" max="9" width="14.5546875" customWidth="true"/>
-    <col min="10" max="10" width="13.5546875" customWidth="true"/>
+    <col min="7" max="7" width="21.44140625" customWidth="true"/>
+    <col min="8" max="8" width="14.5546875" customWidth="true"/>
+    <col min="9" max="9" width="14.21875" customWidth="true"/>
+    <col min="10" max="10" width="14.5546875" customWidth="true"/>
+    <col min="11" max="11" width="13.5546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -127,15 +131,18 @@
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>9</v>
       </c>
     </row>
@@ -159,15 +166,18 @@
         <v>0</v>
       </c>
       <c r="G2" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0">
         <v>1</v>
       </c>
-      <c r="H2" s="0">
-        <v>0</v>
-      </c>
       <c r="I2" s="0">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0">
         <v>0.15183580198325394</v>
       </c>
-      <c r="J2" s="0">
+      <c r="K2" s="0">
         <v>0</v>
       </c>
     </row>
@@ -191,15 +201,18 @@
         <v>0.2084964844357422</v>
       </c>
       <c r="G3" s="0">
+        <v>0.2084964844357422</v>
+      </c>
+      <c r="H3" s="0">
         <v>-0.10046583633758367</v>
       </c>
-      <c r="H3" s="0">
+      <c r="I3" s="0">
         <v>-0.37648694228184698</v>
       </c>
-      <c r="I3" s="0">
+      <c r="J3" s="0">
         <v>-0.10046583633758367</v>
       </c>
-      <c r="J3" s="0">
+      <c r="K3" s="0">
         <v>0.37648694228184698</v>
       </c>
     </row>
@@ -223,15 +236,18 @@
         <v>0.5</v>
       </c>
       <c r="G4" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H4" s="0">
         <v>-0.63703510355648363</v>
       </c>
-      <c r="H4" s="0">
-        <v>0</v>
-      </c>
       <c r="I4" s="0">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0">
         <v>-0.23834762186894135</v>
       </c>
-      <c r="J4" s="0">
+      <c r="K4" s="0">
         <v>0</v>
       </c>
     </row>
@@ -255,15 +271,18 @@
         <v>0.5</v>
       </c>
       <c r="G5" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H5" s="0">
         <v>-0.91790940646609076</v>
       </c>
-      <c r="H5" s="0">
-        <v>0</v>
-      </c>
       <c r="I5" s="0">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0">
         <v>-0.16541480118642488</v>
       </c>
-      <c r="J5" s="0">
+      <c r="K5" s="0">
         <v>0</v>
       </c>
     </row>
@@ -287,15 +306,18 @@
         <v>0.5</v>
       </c>
       <c r="G6" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H6" s="0">
         <v>-0.798648513947672</v>
       </c>
-      <c r="H6" s="0">
-        <v>0</v>
-      </c>
       <c r="I6" s="0">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0">
         <v>-0.19011592624904006</v>
       </c>
-      <c r="J6" s="0">
+      <c r="K6" s="0">
         <v>0</v>
       </c>
     </row>
@@ -319,15 +341,18 @@
         <v>0.56442230618227918</v>
       </c>
       <c r="G7" s="0">
+        <v>0.064422306182279218</v>
+      </c>
+      <c r="H7" s="0">
         <v>-0.35817267042812206</v>
       </c>
-      <c r="H7" s="0">
+      <c r="I7" s="0">
         <v>-0.15345403264355359</v>
       </c>
-      <c r="I7" s="0">
+      <c r="J7" s="0">
         <v>-0.35817267042812206</v>
       </c>
-      <c r="J7" s="0">
+      <c r="K7" s="0">
         <v>0.15345403264355359</v>
       </c>
     </row>
@@ -351,15 +376,18 @@
         <v>0.67390949988399873</v>
       </c>
       <c r="G8" s="0">
+        <v>0.17390949988399879</v>
+      </c>
+      <c r="H8" s="0">
         <v>-0.1792771689613113</v>
       </c>
-      <c r="H8" s="0">
+      <c r="I8" s="0">
         <v>-0.34597037252462826</v>
       </c>
-      <c r="I8" s="0">
+      <c r="J8" s="0">
         <v>-0.1792771689613113</v>
       </c>
-      <c r="J8" s="0">
+      <c r="K8" s="0">
         <v>0.34597037252462826</v>
       </c>
     </row>
@@ -383,15 +411,18 @@
         <v>0.74629623928586053</v>
       </c>
       <c r="G9" s="0">
+        <v>0.2462962392858605</v>
+      </c>
+      <c r="H9" s="0">
         <v>0.0090671475477266655</v>
       </c>
-      <c r="H9" s="0">
+      <c r="I9" s="0">
         <v>-0.38955562993185111</v>
       </c>
-      <c r="I9" s="0">
+      <c r="J9" s="0">
         <v>0.0090671475477266655</v>
       </c>
-      <c r="J9" s="0">
+      <c r="K9" s="0">
         <v>0.38955562993185111</v>
       </c>
     </row>
@@ -415,15 +446,18 @@
         <v>0.82087614050990587</v>
       </c>
       <c r="G10" s="0">
+        <v>0.32087614050990593</v>
+      </c>
+      <c r="H10" s="0">
         <v>0.18402748322967549</v>
       </c>
-      <c r="H10" s="0">
+      <c r="I10" s="0">
         <v>-0.34346715620538232</v>
       </c>
-      <c r="I10" s="0">
+      <c r="J10" s="0">
         <v>0.18402748322967549</v>
       </c>
-      <c r="J10" s="0">
+      <c r="K10" s="0">
         <v>0.34346715620538232</v>
       </c>
     </row>
@@ -447,15 +481,18 @@
         <v>0.90411336088077732</v>
       </c>
       <c r="G11" s="0">
+        <v>0.40411336088077732</v>
+      </c>
+      <c r="H11" s="0">
         <v>0.33098193038826151</v>
       </c>
-      <c r="H11" s="0">
+      <c r="I11" s="0">
         <v>-0.20563745702529312</v>
       </c>
-      <c r="I11" s="0">
+      <c r="J11" s="0">
         <v>0.33098193038826151</v>
       </c>
-      <c r="J11" s="0">
+      <c r="K11" s="0">
         <v>0.20563745702529312</v>
       </c>
     </row>
@@ -479,15 +516,18 @@
         <v>1</v>
       </c>
       <c r="G12" s="0">
+        <v>0</v>
+      </c>
+      <c r="H12" s="0">
         <v>0.23372277871805955</v>
       </c>
-      <c r="H12" s="0">
-        <v>0</v>
-      </c>
       <c r="I12" s="0">
+        <v>0</v>
+      </c>
+      <c r="J12" s="0">
         <v>0.64964058192140795</v>
       </c>
-      <c r="J12" s="0">
+      <c r="K12" s="0">
         <v>0</v>
       </c>
     </row>
@@ -511,15 +551,18 @@
         <v>1</v>
       </c>
       <c r="G13" s="0">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0">
         <v>0.17948344943509181</v>
       </c>
-      <c r="H13" s="0">
-        <v>0</v>
-      </c>
       <c r="I13" s="0">
+        <v>0</v>
+      </c>
+      <c r="J13" s="0">
         <v>0.84595990578347224</v>
       </c>
-      <c r="J13" s="0">
+      <c r="K13" s="0">
         <v>0</v>
       </c>
     </row>
@@ -531,7 +574,7 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="C14" s="0">
-        <v>-0.28746830727795908</v>
+        <v>-0.28746830727795914</v>
       </c>
       <c r="D14" s="0">
         <v>-0.01253169273031411</v>
@@ -543,15 +586,18 @@
         <v>1</v>
       </c>
       <c r="G14" s="0">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0">
         <v>0.16427447130304451</v>
       </c>
-      <c r="H14" s="0">
-        <v>0</v>
-      </c>
       <c r="I14" s="0">
+        <v>0</v>
+      </c>
+      <c r="J14" s="0">
         <v>0.92428117873931748</v>
       </c>
-      <c r="J14" s="0">
+      <c r="K14" s="0">
         <v>0</v>
       </c>
     </row>
@@ -575,15 +621,18 @@
         <v>1</v>
       </c>
       <c r="G15" s="0">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0">
         <v>0.16656244469859244</v>
       </c>
-      <c r="H15" s="0">
-        <v>0</v>
-      </c>
       <c r="I15" s="0">
+        <v>0</v>
+      </c>
+      <c r="J15" s="0">
         <v>0.91158485483792995</v>
       </c>
-      <c r="J15" s="0">
+      <c r="K15" s="0">
         <v>0</v>
       </c>
     </row>
@@ -595,7 +644,7 @@
         <v>1.4000000000000001</v>
       </c>
       <c r="C16" s="0">
-        <v>-0.26789316527092844</v>
+        <v>-0.26789316527092838</v>
       </c>
       <c r="D16" s="0">
         <v>-0.032106834738656505</v>
@@ -607,15 +656,18 @@
         <v>1</v>
       </c>
       <c r="G16" s="0">
+        <v>0</v>
+      </c>
+      <c r="H16" s="0">
         <v>0.18577437115537826</v>
       </c>
-      <c r="H16" s="0">
-        <v>0</v>
-      </c>
       <c r="I16" s="0">
+        <v>0</v>
+      </c>
+      <c r="J16" s="0">
         <v>0.81731296425442945</v>
       </c>
-      <c r="J16" s="0">
+      <c r="K16" s="0">
         <v>0</v>
       </c>
     </row>
@@ -639,15 +691,18 @@
         <v>1</v>
       </c>
       <c r="G17" s="0">
+        <v>0</v>
+      </c>
+      <c r="H17" s="0">
         <v>0.23898016041408932</v>
       </c>
-      <c r="H17" s="0">
-        <v>0</v>
-      </c>
       <c r="I17" s="0">
+        <v>0</v>
+      </c>
+      <c r="J17" s="0">
         <v>0.63534898339726453</v>
       </c>
-      <c r="J17" s="0">
+      <c r="K17" s="0">
         <v>0</v>
       </c>
     </row>
@@ -671,15 +726,18 @@
         <v>1.0706181793689365</v>
       </c>
       <c r="G18" s="0">
+        <v>0.070618179368936496</v>
+      </c>
+      <c r="H18" s="0">
         <v>0.35192886489557218</v>
       </c>
-      <c r="H18" s="0">
+      <c r="I18" s="0">
         <v>-0.16727784080506764</v>
       </c>
-      <c r="I18" s="0">
+      <c r="J18" s="0">
         <v>0.35192886489557218</v>
       </c>
-      <c r="J18" s="0">
+      <c r="K18" s="0">
         <v>0.16727784080506764</v>
       </c>
     </row>
@@ -703,15 +761,18 @@
         <v>1.1381038320827734</v>
       </c>
       <c r="G19" s="0">
+        <v>0.13810383208277344</v>
+      </c>
+      <c r="H19" s="0">
         <v>0.25193868513721807</v>
       </c>
-      <c r="H19" s="0">
+      <c r="I19" s="0">
         <v>-0.29725864310756972</v>
       </c>
-      <c r="I19" s="0">
+      <c r="J19" s="0">
         <v>0.25193868513721807</v>
       </c>
-      <c r="J19" s="0">
+      <c r="K19" s="0">
         <v>0.29725864310756972</v>
       </c>
     </row>
@@ -735,15 +796,18 @@
         <v>1.1901508473357663</v>
       </c>
       <c r="G20" s="0">
+        <v>0.19015084733576623</v>
+      </c>
+      <c r="H20" s="0">
         <v>0.14310038105281237</v>
       </c>
-      <c r="H20" s="0">
+      <c r="I20" s="0">
         <v>-0.3624335565489536</v>
       </c>
-      <c r="I20" s="0">
+      <c r="J20" s="0">
         <v>0.14310038105281237</v>
       </c>
-      <c r="J20" s="0">
+      <c r="K20" s="0">
         <v>0.3624335565489536</v>
       </c>
     </row>
@@ -767,15 +831,18 @@
         <v>1.237364616011237</v>
       </c>
       <c r="G21" s="0">
+        <v>0.23736461601123699</v>
+      </c>
+      <c r="H21" s="0">
         <v>0.030902889986552322</v>
       </c>
-      <c r="H21" s="0">
+      <c r="I21" s="0">
         <v>-0.38843379533759981</v>
       </c>
-      <c r="I21" s="0">
+      <c r="J21" s="0">
         <v>0.030902889986552322</v>
       </c>
-      <c r="J21" s="0">
+      <c r="K21" s="0">
         <v>0.38843379533759981</v>
       </c>
     </row>
@@ -799,15 +866,18 @@
         <v>1.2575281331904664</v>
       </c>
       <c r="G22" s="0">
+        <v>0.25752813319046636</v>
+      </c>
+      <c r="H22" s="0">
         <v>-0.079734787210167274</v>
       </c>
-      <c r="H22" s="0">
+      <c r="I22" s="0">
         <v>-0.38141600081699123</v>
       </c>
-      <c r="I22" s="0">
+      <c r="J22" s="0">
         <v>-0.079734787210167274</v>
       </c>
-      <c r="J22" s="0">
+      <c r="K22" s="0">
         <v>0.38141600081699123</v>
       </c>
     </row>
@@ -831,15 +901,18 @@
         <v>1.3032596311615676</v>
       </c>
       <c r="G23" s="0">
+        <v>0.30325963116156757</v>
+      </c>
+      <c r="H23" s="0">
         <v>-0.18455973747171528</v>
       </c>
-      <c r="H23" s="0">
+      <c r="I23" s="0">
         <v>-0.34318144657735444</v>
       </c>
-      <c r="I23" s="0">
+      <c r="J23" s="0">
         <v>-0.18455973747171528</v>
       </c>
-      <c r="J23" s="0">
+      <c r="K23" s="0">
         <v>0.34318144657735444</v>
       </c>
     </row>
@@ -863,15 +936,18 @@
         <v>1.3523525100006526</v>
       </c>
       <c r="G24" s="0">
+        <v>0.35235251000065249</v>
+      </c>
+      <c r="H24" s="0">
         <v>-0.28003586854368989</v>
       </c>
-      <c r="H24" s="0">
+      <c r="I24" s="0">
         <v>-0.27095334339886851</v>
       </c>
-      <c r="I24" s="0">
+      <c r="J24" s="0">
         <v>-0.28003586854368989</v>
       </c>
-      <c r="J24" s="0">
+      <c r="K24" s="0">
         <v>0.27095334339886851</v>
       </c>
     </row>
@@ -895,15 +971,18 @@
         <v>1.4159174913023511</v>
       </c>
       <c r="G25" s="0">
+        <v>0.41591749130235117</v>
+      </c>
+      <c r="H25" s="0">
         <v>-0.36335861477551368</v>
       </c>
-      <c r="H25" s="0">
+      <c r="I25" s="0">
         <v>-0.14073492472826607</v>
       </c>
-      <c r="I25" s="0">
+      <c r="J25" s="0">
         <v>-0.36335861477551368</v>
       </c>
-      <c r="J25" s="0">
+      <c r="K25" s="0">
         <v>0.14073492472826607</v>
       </c>
     </row>
@@ -927,15 +1006,18 @@
         <v>1.5</v>
       </c>
       <c r="G26" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H26" s="0">
         <v>-0.61997816757496005</v>
       </c>
-      <c r="H26" s="0">
-        <v>0</v>
-      </c>
       <c r="I26" s="0">
+        <v>0</v>
+      </c>
+      <c r="J26" s="0">
         <v>-0.24490507877624987</v>
       </c>
-      <c r="J26" s="0">
+      <c r="K26" s="0">
         <v>0</v>
       </c>
     </row>
@@ -959,15 +1041,18 @@
         <v>1.5</v>
       </c>
       <c r="G27" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H27" s="0">
         <v>-0.77613333504145299</v>
       </c>
-      <c r="H27" s="0">
-        <v>0</v>
-      </c>
       <c r="I27" s="0">
+        <v>0</v>
+      </c>
+      <c r="J27" s="0">
         <v>-0.19563107924088952</v>
       </c>
-      <c r="J27" s="0">
+      <c r="K27" s="0">
         <v>0</v>
       </c>
     </row>
@@ -991,15 +1076,18 @@
         <v>1.5</v>
       </c>
       <c r="G28" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H28" s="0">
         <v>-0.8716237815171437</v>
       </c>
-      <c r="H28" s="0">
-        <v>0</v>
-      </c>
       <c r="I28" s="0">
+        <v>0</v>
+      </c>
+      <c r="J28" s="0">
         <v>-0.17419878299349578</v>
       </c>
-      <c r="J28" s="0">
+      <c r="K28" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1023,15 +1111,18 @@
         <v>1.5</v>
       </c>
       <c r="G29" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H29" s="0">
         <v>-0.92198076696675868</v>
       </c>
-      <c r="H29" s="0">
-        <v>0</v>
-      </c>
       <c r="I29" s="0">
+        <v>0</v>
+      </c>
+      <c r="J29" s="0">
         <v>-0.16468434853303104</v>
       </c>
-      <c r="J29" s="0">
+      <c r="K29" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1055,15 +1146,18 @@
         <v>1.5</v>
       </c>
       <c r="G30" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H30" s="0">
         <v>-0.9319950550808318</v>
       </c>
-      <c r="H30" s="0">
-        <v>0</v>
-      </c>
       <c r="I30" s="0">
+        <v>0</v>
+      </c>
+      <c r="J30" s="0">
         <v>-0.16291481498699634</v>
       </c>
-      <c r="J30" s="0">
+      <c r="K30" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1087,15 +1181,18 @@
         <v>1.5</v>
       </c>
       <c r="G31" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H31" s="0">
         <v>-0.9041016175507357</v>
       </c>
-      <c r="H31" s="0">
-        <v>0</v>
-      </c>
       <c r="I31" s="0">
+        <v>0</v>
+      </c>
+      <c r="J31" s="0">
         <v>-0.16794107987344292</v>
       </c>
-      <c r="J31" s="0">
+      <c r="K31" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1119,15 +1216,18 @@
         <v>1.5</v>
       </c>
       <c r="G32" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H32" s="0">
         <v>-0.83938370625714609</v>
       </c>
-      <c r="H32" s="0">
-        <v>0</v>
-      </c>
       <c r="I32" s="0">
+        <v>0</v>
+      </c>
+      <c r="J32" s="0">
         <v>-0.1808896227488665</v>
       </c>
-      <c r="J32" s="0">
+      <c r="K32" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1151,15 +1251,18 @@
         <v>1.5</v>
       </c>
       <c r="G33" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H33" s="0">
         <v>-0.73613168453932876</v>
       </c>
-      <c r="H33" s="0">
-        <v>0</v>
-      </c>
       <c r="I33" s="0">
+        <v>0</v>
+      </c>
+      <c r="J33" s="0">
         <v>-0.20626173978793544</v>
       </c>
-      <c r="J33" s="0">
+      <c r="K33" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1183,15 +1286,18 @@
         <v>1.5</v>
       </c>
       <c r="G34" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H34" s="0">
         <v>-0.57973429243286712</v>
       </c>
-      <c r="H34" s="0">
-        <v>0</v>
-      </c>
       <c r="I34" s="0">
+        <v>0</v>
+      </c>
+      <c r="J34" s="0">
         <v>-0.26190584884805146</v>
       </c>
-      <c r="J34" s="0">
+      <c r="K34" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1215,15 +1321,18 @@
         <v>1.5616579709366893</v>
       </c>
       <c r="G35" s="0">
+        <v>0.061657970936689309</v>
+      </c>
+      <c r="H35" s="0">
         <v>-0.36078382876454829</v>
       </c>
-      <c r="H35" s="0">
+      <c r="I35" s="0">
         <v>-0.1472101588472568</v>
       </c>
-      <c r="I35" s="0">
+      <c r="J35" s="0">
         <v>-0.36078382876454829</v>
       </c>
-      <c r="J35" s="0">
+      <c r="K35" s="0">
         <v>0.1472101588472568</v>
       </c>
     </row>
@@ -1247,15 +1356,18 @@
         <v>1.6145824315300834</v>
       </c>
       <c r="G36" s="0">
+        <v>0.11458243153008339</v>
+      </c>
+      <c r="H36" s="0">
         <v>-0.29296421025464303</v>
       </c>
-      <c r="H36" s="0">
+      <c r="I36" s="0">
         <v>-0.25691978023411116</v>
       </c>
-      <c r="I36" s="0">
+      <c r="J36" s="0">
         <v>-0.29296421025464303</v>
       </c>
-      <c r="J36" s="0">
+      <c r="K36" s="0">
         <v>0.25691978023411116</v>
       </c>
     </row>
@@ -1279,15 +1391,18 @@
         <v>1.6548712596496185</v>
       </c>
       <c r="G37" s="0">
+        <v>0.15487125964961851</v>
+      </c>
+      <c r="H37" s="0">
         <v>-0.2192826696789022</v>
       </c>
-      <c r="H37" s="0">
+      <c r="I37" s="0">
         <v>-0.32210388501810555</v>
       </c>
-      <c r="I37" s="0">
+      <c r="J37" s="0">
         <v>-0.2192826696789022</v>
       </c>
-      <c r="J37" s="0">
+      <c r="K37" s="0">
         <v>0.32210388501810555</v>
       </c>
     </row>
@@ -1311,15 +1426,18 @@
         <v>1.6907838174164571</v>
       </c>
       <c r="G38" s="0">
+        <v>0.19078381741645709</v>
+      </c>
+      <c r="H38" s="0">
         <v>-0.14165783012446731</v>
       </c>
-      <c r="H38" s="0">
+      <c r="I38" s="0">
         <v>-0.36299980871765747</v>
       </c>
-      <c r="I38" s="0">
+      <c r="J38" s="0">
         <v>-0.14165783012446731</v>
       </c>
-      <c r="J38" s="0">
+      <c r="K38" s="0">
         <v>0.36299980871765747</v>
       </c>
     </row>
@@ -1343,15 +1461,18 @@
         <v>1.7245834799898026</v>
       </c>
       <c r="G39" s="0">
+        <v>0.2245834799898026</v>
+      </c>
+      <c r="H39" s="0">
         <v>-0.061963438005005561</v>
       </c>
-      <c r="H39" s="0">
+      <c r="I39" s="0">
         <v>-0.38470291695764702</v>
       </c>
-      <c r="I39" s="0">
+      <c r="J39" s="0">
         <v>-0.061963438005005561</v>
       </c>
-      <c r="J39" s="0">
+      <c r="K39" s="0">
         <v>0.38470291695764702</v>
       </c>
     </row>
@@ -1375,15 +1496,18 @@
         <v>1.74264225433528</v>
       </c>
       <c r="G40" s="0">
+        <v>0.24264225433527986</v>
+      </c>
+      <c r="H40" s="0">
         <v>0.018007649355113418</v>
       </c>
-      <c r="H40" s="0">
+      <c r="I40" s="0">
         <v>-0.38924481567564018</v>
       </c>
-      <c r="I40" s="0">
+      <c r="J40" s="0">
         <v>0.018007649355113418</v>
       </c>
-      <c r="J40" s="0">
+      <c r="K40" s="0">
         <v>0.38924481567564018</v>
       </c>
     </row>
@@ -1407,15 +1531,18 @@
         <v>1.7751448480488894</v>
       </c>
       <c r="G41" s="0">
+        <v>0.27514484804888939</v>
+      </c>
+      <c r="H41" s="0">
         <v>0.096573556532056529</v>
       </c>
-      <c r="H41" s="0">
+      <c r="I41" s="0">
         <v>-0.37750410612932556</v>
       </c>
-      <c r="I41" s="0">
+      <c r="J41" s="0">
         <v>0.096573556532056529</v>
       </c>
-      <c r="J41" s="0">
+      <c r="K41" s="0">
         <v>0.37750410612932556</v>
       </c>
     </row>
@@ -1439,15 +1566,18 @@
         <v>1.8081306238049981</v>
       </c>
       <c r="G42" s="0">
+        <v>0.30813062380499812</v>
+      </c>
+      <c r="H42" s="0">
         <v>0.17218777830190191</v>
       </c>
-      <c r="H42" s="0">
+      <c r="I42" s="0">
         <v>-0.34955281570674623</v>
       </c>
-      <c r="I42" s="0">
+      <c r="J42" s="0">
         <v>0.17218777830190191</v>
       </c>
-      <c r="J42" s="0">
+      <c r="K42" s="0">
         <v>0.34955281570674623</v>
       </c>
     </row>
@@ -1471,15 +1601,18 @@
         <v>1.8426931474927439</v>
       </c>
       <c r="G43" s="0">
+        <v>0.34269314749274382</v>
+      </c>
+      <c r="H43" s="0">
         <v>0.24345815718378688</v>
       </c>
-      <c r="H43" s="0">
+      <c r="I43" s="0">
         <v>-0.30424320479800271</v>
       </c>
-      <c r="I43" s="0">
+      <c r="J43" s="0">
         <v>0.24345815718378688</v>
       </c>
-      <c r="J43" s="0">
+      <c r="K43" s="0">
         <v>0.30424320479800271</v>
       </c>
     </row>
@@ -1503,15 +1636,18 @@
         <v>1.8811324947788271</v>
       </c>
       <c r="G44" s="0">
+        <v>0.3811324947788271</v>
+      </c>
+      <c r="H44" s="0">
         <v>0.30916080265326829</v>
       </c>
-      <c r="H44" s="0">
+      <c r="I44" s="0">
         <v>-0.2371822085810536</v>
       </c>
-      <c r="I44" s="0">
+      <c r="J44" s="0">
         <v>0.30916080265326829</v>
       </c>
-      <c r="J44" s="0">
+      <c r="K44" s="0">
         <v>0.2371822085810536</v>
       </c>
     </row>
@@ -1535,15 +1671,18 @@
         <v>1.9322782532200171</v>
       </c>
       <c r="G45" s="0">
+        <v>0.43227825322001723</v>
+      </c>
+      <c r="H45" s="0">
         <v>0.36824934607316151</v>
       </c>
-      <c r="H45" s="0">
+      <c r="I45" s="0">
         <v>-0.1273900352506985</v>
       </c>
-      <c r="I45" s="0">
+      <c r="J45" s="0">
         <v>0.36824934607316151</v>
       </c>
-      <c r="J45" s="0">
+      <c r="K45" s="0">
         <v>0.1273900352506985</v>
       </c>
     </row>
@@ -1567,15 +1706,18 @@
         <v>2</v>
       </c>
       <c r="G46" s="0">
+        <v>0</v>
+      </c>
+      <c r="H46" s="0">
         <v>0.26350593837938685</v>
       </c>
-      <c r="H46" s="0">
-        <v>0</v>
-      </c>
       <c r="I46" s="0">
+        <v>0</v>
+      </c>
+      <c r="J46" s="0">
         <v>0.57621396655452162</v>
       </c>
-      <c r="J46" s="0">
+      <c r="K46" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1599,15 +1741,18 @@
         <v>2</v>
       </c>
       <c r="G47" s="0">
+        <v>0</v>
+      </c>
+      <c r="H47" s="0">
         <v>0.21266796803123006</v>
       </c>
-      <c r="H47" s="0">
-        <v>0</v>
-      </c>
       <c r="I47" s="0">
+        <v>0</v>
+      </c>
+      <c r="J47" s="0">
         <v>0.71395708234587696</v>
       </c>
-      <c r="J47" s="0">
+      <c r="K47" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1631,15 +1776,18 @@
         <v>2</v>
       </c>
       <c r="G48" s="0">
+        <v>0</v>
+      </c>
+      <c r="H48" s="0">
         <v>0.18782428765431875</v>
       </c>
-      <c r="H48" s="0">
-        <v>0</v>
-      </c>
       <c r="I48" s="0">
+        <v>0</v>
+      </c>
+      <c r="J48" s="0">
         <v>0.80839280084560572</v>
       </c>
-      <c r="J48" s="0">
+      <c r="K48" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1663,15 +1811,18 @@
         <v>2</v>
       </c>
       <c r="G49" s="0">
+        <v>0</v>
+      </c>
+      <c r="H49" s="0">
         <v>0.17369372996585719</v>
       </c>
-      <c r="H49" s="0">
-        <v>0</v>
-      </c>
       <c r="I49" s="0">
+        <v>0</v>
+      </c>
+      <c r="J49" s="0">
         <v>0.87415822087066775</v>
       </c>
-      <c r="J49" s="0">
+      <c r="K49" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1683,7 +1834,7 @@
         <v>4.8000000000000007</v>
       </c>
       <c r="C50" s="0">
-        <v>-0.28592209889802611</v>
+        <v>-0.28592209889802606</v>
       </c>
       <c r="D50" s="0">
         <v>-0.014077901120465294</v>
@@ -1695,15 +1846,18 @@
         <v>2</v>
       </c>
       <c r="G50" s="0">
+        <v>0</v>
+      </c>
+      <c r="H50" s="0">
         <v>0.16587819404274218</v>
       </c>
-      <c r="H50" s="0">
-        <v>0</v>
-      </c>
       <c r="I50" s="0">
+        <v>0</v>
+      </c>
+      <c r="J50" s="0">
         <v>0.9153451593757046</v>
       </c>
-      <c r="J50" s="0">
+      <c r="K50" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1715,7 +1869,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="C51" s="0">
-        <v>-0.28908734234778033</v>
+        <v>-0.28908734234778027</v>
       </c>
       <c r="D51" s="0">
         <v>-0.010912657671058434</v>
@@ -1727,15 +1881,18 @@
         <v>2</v>
       </c>
       <c r="G51" s="0">
+        <v>0</v>
+      </c>
+      <c r="H51" s="0">
         <v>0.162611827943975</v>
       </c>
-      <c r="H51" s="0">
-        <v>0</v>
-      </c>
       <c r="I51" s="0">
+        <v>0</v>
+      </c>
+      <c r="J51" s="0">
         <v>0.93373159801751216</v>
       </c>
-      <c r="J51" s="0">
+      <c r="K51" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1747,7 +1904,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="0">
-        <v>-0.28850306631269756</v>
+        <v>-0.28850306631269762</v>
       </c>
       <c r="D52" s="0">
         <v>-0.011496933706512606</v>
@@ -1759,15 +1916,18 @@
         <v>2</v>
       </c>
       <c r="G52" s="0">
+        <v>0</v>
+      </c>
+      <c r="H52" s="0">
         <v>0.1632098917081336</v>
       </c>
-      <c r="H52" s="0">
-        <v>0</v>
-      </c>
       <c r="I52" s="0">
+        <v>0</v>
+      </c>
+      <c r="J52" s="0">
         <v>0.9303100466107066</v>
       </c>
-      <c r="J52" s="0">
+      <c r="K52" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1791,15 +1951,18 @@
         <v>2</v>
       </c>
       <c r="G53" s="0">
+        <v>0</v>
+      </c>
+      <c r="H53" s="0">
         <v>0.16764784025073726</v>
       </c>
-      <c r="H53" s="0">
-        <v>0</v>
-      </c>
       <c r="I53" s="0">
+        <v>0</v>
+      </c>
+      <c r="J53" s="0">
         <v>0.90568301825350672</v>
       </c>
-      <c r="J53" s="0">
+      <c r="K53" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1823,15 +1986,18 @@
         <v>2</v>
       </c>
       <c r="G54" s="0">
+        <v>0</v>
+      </c>
+      <c r="H54" s="0">
         <v>0.17654197857465725</v>
       </c>
-      <c r="H54" s="0">
-        <v>0</v>
-      </c>
       <c r="I54" s="0">
+        <v>0</v>
+      </c>
+      <c r="J54" s="0">
         <v>0.86005494663349524</v>
       </c>
-      <c r="J54" s="0">
+      <c r="K54" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1855,15 +2021,18 @@
         <v>2</v>
       </c>
       <c r="G55" s="0">
+        <v>0</v>
+      </c>
+      <c r="H55" s="0">
         <v>0.19150744770999673</v>
       </c>
-      <c r="H55" s="0">
-        <v>0</v>
-      </c>
       <c r="I55" s="0">
+        <v>0</v>
+      </c>
+      <c r="J55" s="0">
         <v>0.79284541555407318</v>
       </c>
-      <c r="J55" s="0">
+      <c r="K55" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1887,15 +2056,18 @@
         <v>2</v>
       </c>
       <c r="G56" s="0">
+        <v>0</v>
+      </c>
+      <c r="H56" s="0">
         <v>0.21650102135577498</v>
       </c>
-      <c r="H56" s="0">
-        <v>0</v>
-      </c>
       <c r="I56" s="0">
+        <v>0</v>
+      </c>
+      <c r="J56" s="0">
         <v>0.70131679291988247</v>
       </c>
-      <c r="J56" s="0">
+      <c r="K56" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1910,7 +2082,7 @@
         <v>-0.21156827611741144</v>
       </c>
       <c r="D57" s="0">
-        <v>-0.088431723903173359</v>
+        <v>-0.088431723903173346</v>
       </c>
       <c r="E57" s="0">
         <v>-2</v>
@@ -1919,15 +2091,18 @@
         <v>2</v>
       </c>
       <c r="G57" s="0">
+        <v>0</v>
+      </c>
+      <c r="H57" s="0">
         <v>0.26465645666856663</v>
       </c>
-      <c r="H57" s="0">
-        <v>0</v>
-      </c>
       <c r="I57" s="0">
+        <v>0</v>
+      </c>
+      <c r="J57" s="0">
         <v>0.57370904104242981</v>
       </c>
-      <c r="J57" s="0">
+      <c r="K57" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1951,15 +2126,18 @@
         <v>2.0456424087731899</v>
       </c>
       <c r="G58" s="0">
+        <v>0.045642408773189827</v>
+      </c>
+      <c r="H58" s="0">
         <v>0.37374728055620532</v>
       </c>
-      <c r="H58" s="0">
+      <c r="I58" s="0">
         <v>-0.11022146904178964</v>
       </c>
-      <c r="I58" s="0">
+      <c r="J58" s="0">
         <v>0.37374728055620532</v>
       </c>
-      <c r="J58" s="0">
+      <c r="K58" s="0">
         <v>0.11022146904178964</v>
       </c>
     </row>
@@ -1983,15 +2161,18 @@
         <v>2.0941840722044463</v>
       </c>
       <c r="G59" s="0">
+        <v>0.094184072204446232</v>
+      </c>
+      <c r="H59" s="0">
         <v>0.32339976122510383</v>
       </c>
-      <c r="H59" s="0">
+      <c r="I59" s="0">
         <v>-0.2173669625316676</v>
       </c>
-      <c r="I59" s="0">
+      <c r="J59" s="0">
         <v>0.32339976122510383</v>
       </c>
-      <c r="J59" s="0">
+      <c r="K59" s="0">
         <v>0.2173669625316676</v>
       </c>
     </row>
@@ -2015,15 +2196,18 @@
         <v>2.1287459110969538</v>
       </c>
       <c r="G60" s="0">
+        <v>0.12874591109695357</v>
+      </c>
+      <c r="H60" s="0">
         <v>0.26897132683349434</v>
       </c>
-      <c r="H60" s="0">
+      <c r="I60" s="0">
         <v>-0.28194011297076638</v>
       </c>
-      <c r="I60" s="0">
+      <c r="J60" s="0">
         <v>0.26897132683349434</v>
       </c>
-      <c r="J60" s="0">
+      <c r="K60" s="0">
         <v>0.28194011297076638</v>
       </c>
     </row>
@@ -2047,15 +2231,18 @@
         <v>2.1587766586525121</v>
       </c>
       <c r="G61" s="0">
+        <v>0.15877665865251195</v>
+      </c>
+      <c r="H61" s="0">
         <v>0.21131355131816226</v>
       </c>
-      <c r="H61" s="0">
+      <c r="I61" s="0">
         <v>-0.32738720956931278</v>
       </c>
-      <c r="I61" s="0">
+      <c r="J61" s="0">
         <v>0.21131355131816226</v>
       </c>
-      <c r="J61" s="0">
+      <c r="K61" s="0">
         <v>0.32738720956931278</v>
       </c>
     </row>
@@ -2079,15 +2266,18 @@
         <v>2.1865399350500554</v>
       </c>
       <c r="G62" s="0">
+        <v>0.18653993505005526</v>
+      </c>
+      <c r="H62" s="0">
         <v>0.15128575073876888</v>
       </c>
-      <c r="H62" s="0">
+      <c r="I62" s="0">
         <v>-0.35909389243405382</v>
       </c>
-      <c r="I62" s="0">
+      <c r="J62" s="0">
         <v>0.15128575073876888</v>
       </c>
-      <c r="J62" s="0">
+      <c r="K62" s="0">
         <v>0.35909389243405382</v>
       </c>
     </row>
@@ -2111,15 +2301,18 @@
         <v>2.2130128751414526</v>
       </c>
       <c r="G63" s="0">
+        <v>0.2130128751414527</v>
+      </c>
+      <c r="H63" s="0">
         <v>0.089743131359107969</v>
       </c>
-      <c r="H63" s="0">
+      <c r="I63" s="0">
         <v>-0.37918593372310705</v>
       </c>
-      <c r="I63" s="0">
+      <c r="J63" s="0">
         <v>0.089743131359107969</v>
       </c>
-      <c r="J63" s="0">
+      <c r="K63" s="0">
         <v>0.37918593372310705</v>
       </c>
     </row>
@@ -2143,15 +2336,18 @@
         <v>2.2387478425018879</v>
       </c>
       <c r="G64" s="0">
+        <v>0.23874784250188769</v>
+      </c>
+      <c r="H64" s="0">
         <v>0.027525860703066792</v>
       </c>
-      <c r="H64" s="0">
+      <c r="I64" s="0">
         <v>-0.38868770105616435</v>
       </c>
-      <c r="I64" s="0">
+      <c r="J64" s="0">
         <v>0.027525860703066792</v>
       </c>
-      <c r="J64" s="0">
+      <c r="K64" s="0">
         <v>0.38868770105616435</v>
       </c>
     </row>
@@ -2175,15 +2371,18 @@
         <v>2.2416263589972223</v>
       </c>
       <c r="G65" s="0">
+        <v>0.2416263589972224</v>
+      </c>
+      <c r="H65" s="0">
         <v>-0.034550879467842119</v>
       </c>
-      <c r="H65" s="0">
+      <c r="I65" s="0">
         <v>-0.38812631795321184</v>
       </c>
-      <c r="I65" s="0">
+      <c r="J65" s="0">
         <v>-0.034550879467842119</v>
       </c>
-      <c r="J65" s="0">
+      <c r="K65" s="0">
         <v>0.38812631795321184</v>
       </c>
     </row>
@@ -2207,15 +2406,18 @@
         <v>2.2669902947103426</v>
       </c>
       <c r="G66" s="0">
+        <v>0.26699029471034263</v>
+      </c>
+      <c r="H66" s="0">
         <v>-0.095705817771178092</v>
       </c>
-      <c r="H66" s="0">
+      <c r="I66" s="0">
         <v>-0.37772503015428505</v>
       </c>
-      <c r="I66" s="0">
+      <c r="J66" s="0">
         <v>-0.095705817771178092</v>
       </c>
-      <c r="J66" s="0">
+      <c r="K66" s="0">
         <v>0.37772503015428505</v>
       </c>
     </row>
@@ -2239,15 +2441,18 @@
         <v>2.2926943959592245</v>
       </c>
       <c r="G67" s="0">
+        <v>0.29269439595922458</v>
+      </c>
+      <c r="H67" s="0">
         <v>-0.15519947174732918</v>
       </c>
-      <c r="H67" s="0">
+      <c r="I67" s="0">
         <v>-0.3574198174827154</v>
       </c>
-      <c r="I67" s="0">
+      <c r="J67" s="0">
         <v>-0.15519947174732918</v>
       </c>
-      <c r="J67" s="0">
+      <c r="K67" s="0">
         <v>0.3574198174827154</v>
       </c>
     </row>
@@ -2271,15 +2476,18 @@
         <v>2.3192190009003659</v>
       </c>
       <c r="G68" s="0">
+        <v>0.31921900090036592</v>
+      </c>
+      <c r="H68" s="0">
         <v>-0.2123409718416108</v>
       </c>
-      <c r="H68" s="0">
+      <c r="I68" s="0">
         <v>-0.32672176792636776</v>
       </c>
-      <c r="I68" s="0">
+      <c r="J68" s="0">
         <v>-0.2123409718416108</v>
       </c>
-      <c r="J68" s="0">
+      <c r="K68" s="0">
         <v>0.32672176792636776</v>
       </c>
     </row>
@@ -2291,10 +2499,10 @@
         <v>6.7000000000000002</v>
       </c>
       <c r="C69" s="0">
-        <v>-0.15000000001108618</v>
+        <v>-0.15000000001108615</v>
       </c>
       <c r="D69" s="0">
-        <v>-0.15000000001108618</v>
+        <v>-0.15000000001108615</v>
       </c>
       <c r="E69" s="0">
         <v>-2.3473570282268783</v>
@@ -2303,15 +2511,18 @@
         <v>2.3473570282268783</v>
       </c>
       <c r="G69" s="0">
+        <v>0.34735702822687842</v>
+      </c>
+      <c r="H69" s="0">
         <v>-0.26649383589119391</v>
       </c>
-      <c r="H69" s="0">
+      <c r="I69" s="0">
         <v>-0.28428302339656803</v>
       </c>
-      <c r="I69" s="0">
+      <c r="J69" s="0">
         <v>-0.26649383589119391</v>
       </c>
-      <c r="J69" s="0">
+      <c r="K69" s="0">
         <v>0.28428302339656803</v>
       </c>
     </row>
@@ -2335,15 +2546,18 @@
         <v>2.3787801953495236</v>
       </c>
       <c r="G70" s="0">
+        <v>0.3787801953495234</v>
+      </c>
+      <c r="H70" s="0">
         <v>-0.31708071117515446</v>
       </c>
-      <c r="H70" s="0">
+      <c r="I70" s="0">
         <v>-0.22648537383277115</v>
       </c>
-      <c r="I70" s="0">
+      <c r="J70" s="0">
         <v>-0.31708071117515446</v>
       </c>
-      <c r="J70" s="0">
+      <c r="K70" s="0">
         <v>0.22648537383277115</v>
       </c>
     </row>
@@ -2367,15 +2581,18 @@
         <v>2.4189428917711808</v>
       </c>
       <c r="G71" s="0">
+        <v>0.41894289177118094</v>
+      </c>
+      <c r="H71" s="0">
         <v>-0.36358711156508583</v>
       </c>
-      <c r="H71" s="0">
+      <c r="I71" s="0">
         <v>-0.140143548774712</v>
       </c>
-      <c r="I71" s="0">
+      <c r="J71" s="0">
         <v>-0.36358711156508583</v>
       </c>
-      <c r="J71" s="0">
+      <c r="K71" s="0">
         <v>0.140143548774712</v>
       </c>
     </row>
@@ -2399,15 +2616,18 @@
         <v>2.5</v>
       </c>
       <c r="G72" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H72" s="0">
         <v>-0.51802087698752786</v>
       </c>
-      <c r="H72" s="0">
-        <v>0</v>
-      </c>
       <c r="I72" s="0">
+        <v>0</v>
+      </c>
+      <c r="J72" s="0">
         <v>-0.29310749567129502</v>
       </c>
-      <c r="J72" s="0">
+      <c r="K72" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2431,15 +2651,18 @@
         <v>2.5</v>
       </c>
       <c r="G73" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H73" s="0">
         <v>-0.6525972643607193</v>
       </c>
-      <c r="H73" s="0">
-        <v>0</v>
-      </c>
       <c r="I73" s="0">
+        <v>0</v>
+      </c>
+      <c r="J73" s="0">
         <v>-0.23266386522148236</v>
       </c>
-      <c r="J73" s="0">
+      <c r="K73" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2463,15 +2686,18 @@
         <v>2.5</v>
       </c>
       <c r="G74" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H74" s="0">
         <v>-0.74519299131551464</v>
       </c>
-      <c r="H74" s="0">
-        <v>0</v>
-      </c>
       <c r="I74" s="0">
+        <v>0</v>
+      </c>
+      <c r="J74" s="0">
         <v>-0.20375366345147267</v>
       </c>
-      <c r="J74" s="0">
+      <c r="K74" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2495,15 +2721,18 @@
         <v>2.5</v>
       </c>
       <c r="G75" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H75" s="0">
         <v>-0.81551159197165912</v>
       </c>
-      <c r="H75" s="0">
-        <v>0</v>
-      </c>
       <c r="I75" s="0">
+        <v>0</v>
+      </c>
+      <c r="J75" s="0">
         <v>-0.18618472558014704</v>
       </c>
-      <c r="J75" s="0">
+      <c r="K75" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2527,15 +2756,18 @@
         <v>2.5</v>
       </c>
       <c r="G76" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H76" s="0">
         <v>-0.86828983703360008</v>
       </c>
-      <c r="H76" s="0">
-        <v>0</v>
-      </c>
       <c r="I76" s="0">
+        <v>0</v>
+      </c>
+      <c r="J76" s="0">
         <v>-0.17486764843072522</v>
       </c>
-      <c r="J76" s="0">
+      <c r="K76" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2559,15 +2791,18 @@
         <v>2.5</v>
       </c>
       <c r="G77" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H77" s="0">
         <v>-0.9054131047441244</v>
       </c>
-      <c r="H77" s="0">
-        <v>0</v>
-      </c>
       <c r="I77" s="0">
+        <v>0</v>
+      </c>
+      <c r="J77" s="0">
         <v>-0.16769781789386867</v>
       </c>
-      <c r="J77" s="0">
+      <c r="K77" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2591,15 +2826,18 @@
         <v>2.5</v>
       </c>
       <c r="G78" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H78" s="0">
         <v>-0.92781880791810689</v>
       </c>
-      <c r="H78" s="0">
-        <v>0</v>
-      </c>
       <c r="I78" s="0">
+        <v>0</v>
+      </c>
+      <c r="J78" s="0">
         <v>-0.16364811821235015</v>
       </c>
-      <c r="J78" s="0">
+      <c r="K78" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2623,15 +2861,18 @@
         <v>2.5</v>
       </c>
       <c r="G79" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H79" s="0">
         <v>-0.93605152347479537</v>
       </c>
-      <c r="H79" s="0">
-        <v>0</v>
-      </c>
       <c r="I79" s="0">
+        <v>0</v>
+      </c>
+      <c r="J79" s="0">
         <v>-0.16220880811551702</v>
       </c>
-      <c r="J79" s="0">
+      <c r="K79" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2655,15 +2896,18 @@
         <v>2.5</v>
       </c>
       <c r="G80" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H80" s="0">
         <v>-0.93046112979057793</v>
       </c>
-      <c r="H80" s="0">
-        <v>0</v>
-      </c>
       <c r="I80" s="0">
+        <v>0</v>
+      </c>
+      <c r="J80" s="0">
         <v>-0.16318339057483505</v>
       </c>
-      <c r="J80" s="0">
+      <c r="K80" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2687,15 +2931,18 @@
         <v>2.5</v>
       </c>
       <c r="G81" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H81" s="0">
         <v>-0.91126334932609399</v>
       </c>
-      <c r="H81" s="0">
-        <v>0</v>
-      </c>
       <c r="I81" s="0">
+        <v>0</v>
+      </c>
+      <c r="J81" s="0">
         <v>-0.16662121006977954</v>
       </c>
-      <c r="J81" s="0">
+      <c r="K81" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2719,15 +2966,18 @@
         <v>2.5</v>
       </c>
       <c r="G82" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H82" s="0">
         <v>-0.87851781924213757</v>
       </c>
-      <c r="H82" s="0">
-        <v>0</v>
-      </c>
       <c r="I82" s="0">
+        <v>0</v>
+      </c>
+      <c r="J82" s="0">
         <v>-0.17283178397865767</v>
       </c>
-      <c r="J82" s="0">
+      <c r="K82" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2751,15 +3001,18 @@
         <v>2.5</v>
       </c>
       <c r="G83" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H83" s="0">
         <v>-0.83201246389187267</v>
       </c>
-      <c r="H83" s="0">
-        <v>0</v>
-      </c>
       <c r="I83" s="0">
+        <v>0</v>
+      </c>
+      <c r="J83" s="0">
         <v>-0.18249222042440255</v>
       </c>
-      <c r="J83" s="0">
+      <c r="K83" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2783,15 +3036,18 @@
         <v>2.5</v>
       </c>
       <c r="G84" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H84" s="0">
         <v>-0.77095758385264457</v>
       </c>
-      <c r="H84" s="0">
-        <v>0</v>
-      </c>
       <c r="I84" s="0">
+        <v>0</v>
+      </c>
+      <c r="J84" s="0">
         <v>-0.19694443006506229</v>
       </c>
-      <c r="J84" s="0">
+      <c r="K84" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2815,15 +3071,18 @@
         <v>2.5</v>
       </c>
       <c r="G85" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H85" s="0">
         <v>-0.69310620055623384</v>
       </c>
-      <c r="H85" s="0">
-        <v>0</v>
-      </c>
       <c r="I85" s="0">
+        <v>0</v>
+      </c>
+      <c r="J85" s="0">
         <v>-0.21906571003723224</v>
       </c>
-      <c r="J85" s="0">
+      <c r="K85" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2847,15 +3106,18 @@
         <v>2.5</v>
       </c>
       <c r="G86" s="0">
+        <v>-0</v>
+      </c>
+      <c r="H86" s="0">
         <v>-0.59117703243383701</v>
       </c>
-      <c r="H86" s="0">
-        <v>0</v>
-      </c>
       <c r="I86" s="0">
+        <v>0</v>
+      </c>
+      <c r="J86" s="0">
         <v>-0.25683643583180726</v>
       </c>
-      <c r="J86" s="0">
+      <c r="K86" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2879,15 +3141,18 @@
         <v>2.5142854479217793</v>
       </c>
       <c r="G87" s="0">
+        <v>0.014285447921779524</v>
+      </c>
+      <c r="H87" s="0">
         <v>-0.38809253462013338</v>
       </c>
-      <c r="H87" s="0">
+      <c r="I87" s="0">
         <v>-0.034928305540963357</v>
       </c>
-      <c r="I87" s="0">
+      <c r="J87" s="0">
         <v>-0.38809253462013338</v>
       </c>
-      <c r="J87" s="0">
+      <c r="K87" s="0">
         <v>0.034928305540963357</v>
       </c>
     </row>
@@ -2911,15 +3176,18 @@
         <v>2.5735870515762405</v>
       </c>
       <c r="G88" s="0">
+        <v>0.073587051576240445</v>
+      </c>
+      <c r="H88" s="0">
         <v>-0.34874742060978281</v>
       </c>
-      <c r="H88" s="0">
+      <c r="I88" s="0">
         <v>-0.17381322899519333</v>
       </c>
-      <c r="I88" s="0">
+      <c r="J88" s="0">
         <v>-0.34874742060978281</v>
       </c>
-      <c r="J88" s="0">
+      <c r="K88" s="0">
         <v>0.17381322899519333</v>
       </c>
     </row>
@@ -2943,15 +3211,18 @@
         <v>2.6059936996249538</v>
       </c>
       <c r="G89" s="0">
+        <v>0.10599369962495382</v>
+      </c>
+      <c r="H89" s="0">
         <v>-0.30639557517034099</v>
       </c>
-      <c r="H89" s="0">
+      <c r="I89" s="0">
         <v>-0.24074375063867559</v>
       </c>
-      <c r="I89" s="0">
+      <c r="J89" s="0">
         <v>-0.30639557517034099</v>
       </c>
-      <c r="J89" s="0">
+      <c r="K89" s="0">
         <v>0.24074375063867559</v>
       </c>
     </row>
@@ -2975,15 +3246,18 @@
         <v>2.6329248177591871</v>
       </c>
       <c r="G90" s="0">
+        <v>0.13292481775918694</v>
+      </c>
+      <c r="H90" s="0">
         <v>-0.2614766075506314</v>
       </c>
-      <c r="H90" s="0">
+      <c r="I90" s="0">
         <v>-0.28890445766580192</v>
       </c>
-      <c r="I90" s="0">
+      <c r="J90" s="0">
         <v>-0.2614766075506314</v>
       </c>
-      <c r="J90" s="0">
+      <c r="K90" s="0">
         <v>0.28890445766580192</v>
       </c>
     </row>
@@ -3007,15 +3281,18 @@
         <v>2.6572515711374023</v>
       </c>
       <c r="G91" s="0">
+        <v>0.15725157113740235</v>
+      </c>
+      <c r="H91" s="0">
         <v>-0.2144409593475381</v>
       </c>
-      <c r="H91" s="0">
+      <c r="I91" s="0">
         <v>-0.32534731735366362</v>
       </c>
-      <c r="I91" s="0">
+      <c r="J91" s="0">
         <v>-0.2144409593475381</v>
       </c>
-      <c r="J91" s="0">
+      <c r="K91" s="0">
         <v>0.32534731735366362</v>
       </c>
     </row>
@@ -3039,15 +3316,18 @@
         <v>2.6800741119027061</v>
       </c>
       <c r="G92" s="0">
+        <v>0.18007411190270628</v>
+      </c>
+      <c r="H92" s="0">
         <v>-0.16574544493135859</v>
       </c>
-      <c r="H92" s="0">
+      <c r="I92" s="0">
         <v>-0.35265315742136444</v>
       </c>
-      <c r="I92" s="0">
+      <c r="J92" s="0">
         <v>-0.16574544493135859</v>
       </c>
-      <c r="J92" s="0">
+      <c r="K92" s="0">
         <v>0.35265315742136444</v>
       </c>
     </row>

</xml_diff>